<commit_message>
Update few lines of code
</commit_message>
<xml_diff>
--- a/data/mcgo_summary.xlsx
+++ b/data/mcgo_summary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +54,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,9 +405,9 @@
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1990</v>
       </c>
@@ -435,7 +435,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1991</v>
       </c>
@@ -449,7 +449,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1992</v>
       </c>
@@ -463,7 +463,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>1993</v>
       </c>
@@ -477,7 +477,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>1994</v>
       </c>
@@ -491,7 +491,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>1995</v>
       </c>
@@ -505,7 +505,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>1996</v>
       </c>
@@ -519,7 +519,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>1997</v>
       </c>
@@ -533,7 +533,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>1998</v>
       </c>
@@ -547,7 +547,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>1999</v>
       </c>
@@ -561,7 +561,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>2000</v>
       </c>
@@ -575,7 +575,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>2001</v>
       </c>
@@ -589,7 +589,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -603,7 +603,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -617,7 +617,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>2004</v>
       </c>
@@ -631,7 +631,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>2005</v>
       </c>
@@ -645,7 +645,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>2006</v>
       </c>
@@ -659,7 +659,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>2007</v>
       </c>
@@ -673,7 +673,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>2008</v>
       </c>
@@ -687,7 +687,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>2009</v>
       </c>
@@ -701,7 +701,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>2010</v>
       </c>
@@ -715,7 +715,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -729,7 +729,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>2012</v>
       </c>
@@ -743,7 +743,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>2013</v>
       </c>
@@ -757,7 +757,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>2014</v>
       </c>
@@ -771,7 +771,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>2015</v>
       </c>
@@ -785,7 +785,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>2016</v>
       </c>
@@ -799,7 +799,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>2017</v>
       </c>
@@ -813,7 +813,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>2018</v>
       </c>
@@ -827,7 +827,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -841,7 +841,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -855,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>2021</v>
       </c>
@@ -869,7 +869,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>2022</v>
       </c>
@@ -883,7 +883,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>2023</v>
       </c>
@@ -897,7 +897,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>2024</v>
       </c>

</xml_diff>

<commit_message>
update r script to include coordinates in tables 1 and 2
</commit_message>
<xml_diff>
--- a/data/mcgo_summary.xlsx
+++ b/data/mcgo_summary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfriendly\Desktop\cackler\data\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfriendly\OneDrive - DOI\Desktop\cackler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603F81BB-5297-4EEF-A8FC-E838ACE7AB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8B76ED-81CD-4A7A-964E-997131ECE306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="4050" windowWidth="29040" windowHeight="15840" xr2:uid="{EF7F45EA-C232-436D-B295-54EAED5BAF44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{EF7F45EA-C232-436D-B295-54EAED5BAF44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t>Year</t>
   </si>
@@ -49,12 +50,15 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,9 +107,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -143,7 +147,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -249,7 +253,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -391,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -399,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B6A64F-7402-4EEB-A071-297C2B6626AD}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1990</v>
       </c>
@@ -435,7 +439,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1991</v>
       </c>
@@ -449,7 +453,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1992</v>
       </c>
@@ -463,7 +467,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1993</v>
       </c>
@@ -477,7 +481,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1994</v>
       </c>
@@ -491,7 +495,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1995</v>
       </c>
@@ -505,7 +509,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1996</v>
       </c>
@@ -519,7 +523,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1997</v>
       </c>
@@ -533,7 +537,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1998</v>
       </c>
@@ -547,7 +551,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1999</v>
       </c>
@@ -561,7 +565,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2000</v>
       </c>
@@ -575,7 +579,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2001</v>
       </c>
@@ -589,7 +593,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -603,7 +607,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -617,7 +621,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2004</v>
       </c>
@@ -631,7 +635,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2005</v>
       </c>
@@ -645,7 +649,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2006</v>
       </c>
@@ -659,7 +663,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2007</v>
       </c>
@@ -673,7 +677,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2008</v>
       </c>
@@ -687,7 +691,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2009</v>
       </c>
@@ -701,7 +705,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2010</v>
       </c>
@@ -715,7 +719,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2011</v>
       </c>
@@ -729,7 +733,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2012</v>
       </c>
@@ -743,7 +747,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2013</v>
       </c>
@@ -757,7 +761,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2014</v>
       </c>
@@ -771,7 +775,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2015</v>
       </c>
@@ -785,7 +789,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2016</v>
       </c>
@@ -799,7 +803,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2017</v>
       </c>
@@ -813,7 +817,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2018</v>
       </c>
@@ -827,7 +831,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -841,7 +845,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -855,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2021</v>
       </c>
@@ -869,7 +873,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2022</v>
       </c>
@@ -883,7 +887,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2023</v>
       </c>
@@ -897,7 +901,593 @@
         <v>885</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2024</v>
+      </c>
+      <c r="B36">
+        <v>669</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2025</v>
+      </c>
+      <c r="B37">
+        <v>1168</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6760960B-B1EE-456D-B81C-5114B82CEA12}">
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="2.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1990</v>
+      </c>
+      <c r="B2">
+        <v>285</v>
+      </c>
+      <c r="C2">
+        <v>289</v>
+      </c>
+      <c r="D2">
+        <v>574</v>
+      </c>
+      <c r="F2">
+        <v>2025</v>
+      </c>
+      <c r="G2">
+        <v>1168</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1991</v>
+      </c>
+      <c r="B3">
+        <v>376</v>
+      </c>
+      <c r="C3">
+        <v>274</v>
+      </c>
+      <c r="D3">
+        <v>650</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f>SUM(B2:B35,G2)</f>
+        <v>15719</v>
+      </c>
+      <c r="H3">
+        <f>SUM(C2:C36,H2)</f>
+        <v>10191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1992</v>
+      </c>
+      <c r="B4">
+        <v>235</v>
+      </c>
+      <c r="C4">
+        <v>366</v>
+      </c>
+      <c r="D4">
+        <v>601</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <f>AVERAGE(B2:B36,G2)</f>
+        <v>455.22222222222223</v>
+      </c>
+      <c r="H4">
+        <f>AVERAGE(C2:C36,H2)</f>
+        <v>283.08333333333331</v>
+      </c>
+      <c r="I4">
+        <f>AVERAGE(D2:D36,I2)</f>
+        <v>738.30555555555554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1993</v>
+      </c>
+      <c r="B5">
+        <v>284</v>
+      </c>
+      <c r="C5">
+        <v>490</v>
+      </c>
+      <c r="D5">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1994</v>
+      </c>
+      <c r="B6">
+        <v>342</v>
+      </c>
+      <c r="C6">
+        <v>629</v>
+      </c>
+      <c r="D6">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1995</v>
+      </c>
+      <c r="B7">
+        <v>129</v>
+      </c>
+      <c r="C7">
+        <v>1183</v>
+      </c>
+      <c r="D7">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1996</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>466</v>
+      </c>
+      <c r="D8">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1997</v>
+      </c>
+      <c r="B9">
+        <v>284</v>
+      </c>
+      <c r="C9">
+        <v>772</v>
+      </c>
+      <c r="D9">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1998</v>
+      </c>
+      <c r="B10">
+        <v>313</v>
+      </c>
+      <c r="C10">
+        <v>1058</v>
+      </c>
+      <c r="D10">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1999</v>
+      </c>
+      <c r="B11">
+        <v>250</v>
+      </c>
+      <c r="C11">
+        <v>633</v>
+      </c>
+      <c r="D11">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2000</v>
+      </c>
+      <c r="B12">
+        <v>320</v>
+      </c>
+      <c r="C12">
+        <v>386</v>
+      </c>
+      <c r="D12">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2001</v>
+      </c>
+      <c r="B13">
+        <v>413</v>
+      </c>
+      <c r="C13">
+        <v>292</v>
+      </c>
+      <c r="D13">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2002</v>
+      </c>
+      <c r="B14">
+        <v>260</v>
+      </c>
+      <c r="C14">
+        <v>429</v>
+      </c>
+      <c r="D14">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2003</v>
+      </c>
+      <c r="B15">
+        <v>500</v>
+      </c>
+      <c r="C15">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2004</v>
+      </c>
+      <c r="B16">
+        <v>170</v>
+      </c>
+      <c r="C16">
+        <v>607</v>
+      </c>
+      <c r="D16">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2005</v>
+      </c>
+      <c r="B17">
+        <v>884</v>
+      </c>
+      <c r="C17">
+        <v>498</v>
+      </c>
+      <c r="D17">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2006</v>
+      </c>
+      <c r="B18">
+        <v>235</v>
+      </c>
+      <c r="C18">
+        <v>104</v>
+      </c>
+      <c r="D18">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2007</v>
+      </c>
+      <c r="B19">
+        <v>594</v>
+      </c>
+      <c r="C19">
+        <v>407</v>
+      </c>
+      <c r="D19">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2008</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>557</v>
+      </c>
+      <c r="D20">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2009</v>
+      </c>
+      <c r="B21">
+        <v>363</v>
+      </c>
+      <c r="C21">
+        <v>372</v>
+      </c>
+      <c r="D21">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2010</v>
+      </c>
+      <c r="B22">
+        <v>385</v>
+      </c>
+      <c r="C22">
+        <v>356</v>
+      </c>
+      <c r="D22">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2011</v>
+      </c>
+      <c r="B23">
+        <v>1352</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2012</v>
+      </c>
+      <c r="B24">
+        <v>1035</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2013</v>
+      </c>
+      <c r="B25">
+        <v>1057</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2014</v>
+      </c>
+      <c r="B26">
+        <v>176</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2015</v>
+      </c>
+      <c r="B27">
+        <v>117</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2016</v>
+      </c>
+      <c r="B28">
+        <v>288</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2017</v>
+      </c>
+      <c r="B29">
+        <v>429</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2018</v>
+      </c>
+      <c r="B30">
+        <v>490</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2019</v>
+      </c>
+      <c r="B31">
+        <v>551</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>2020</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2021</v>
+      </c>
+      <c r="B33">
+        <v>781</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2022</v>
+      </c>
+      <c r="B34">
+        <v>768</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2023</v>
+      </c>
+      <c r="B35">
+        <v>885</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2024</v>
       </c>

</xml_diff>